<commit_message>
Unreal Polishing Game Flow
</commit_message>
<xml_diff>
--- a/Unreal_Part2/ArenaBattle/GameData/ABCharacterStatTable.xlsx
+++ b/Unreal_Part2/ArenaBattle/GameData/ABCharacterStatTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UE5Part2\PreTest\ArenaBattle10pre\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnrealTest\Unreal_Study\Unreal_Part2\ArenaBattle\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6DBFFE-125E-4A66-AF5B-85CEEB9F49AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE807F19-4E62-41BD-BFE5-C8C3BAD8ED37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="1120" windowWidth="31540" windowHeight="17940" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
+    <workbookView xWindow="3420" yWindow="1950" windowWidth="14640" windowHeight="14050" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -133,7 +133,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -448,7 +448,7 @@
   <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -486,7 +486,7 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <v>40</v>
@@ -506,7 +506,7 @@
         <v>150</v>
       </c>
       <c r="C4" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1">
         <v>40</v>
@@ -526,7 +526,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="1">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D5" s="1">
         <v>40</v>
@@ -566,7 +566,7 @@
         <v>300</v>
       </c>
       <c r="C7" s="1">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D7" s="1">
         <v>40</v>
@@ -586,7 +586,7 @@
         <v>350</v>
       </c>
       <c r="C8" s="1">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="D8" s="1">
         <v>40</v>
@@ -606,7 +606,7 @@
         <v>400</v>
       </c>
       <c r="C9" s="1">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D9" s="1">
         <v>40</v>
@@ -626,7 +626,7 @@
         <v>450</v>
       </c>
       <c r="C10" s="1">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="D10" s="1">
         <v>40</v>
@@ -646,7 +646,7 @@
         <v>500</v>
       </c>
       <c r="C11" s="1">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D11" s="1">
         <v>40</v>
@@ -666,7 +666,7 @@
         <v>550</v>
       </c>
       <c r="C12" s="1">
-        <v>280</v>
+        <v>400</v>
       </c>
       <c r="D12" s="1">
         <v>40</v>
@@ -681,5 +681,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>